<commit_message>
added import file controller
</commit_message>
<xml_diff>
--- a/backend/src/test/resources/output/testExcelColumnName.xlsx
+++ b/backend/src/test/resources/output/testExcelColumnName.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Montant</t>
-  </si>
-  <si>
-    <t>biteme</t>
   </si>
 </sst>
 </file>
@@ -77,36 +74,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A1"/>
+      <c r="B1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>